<commit_message>
Fixed Weapon Spec: Maul bug
Fixed Weapon Spec: Maul bug, updated skill changes notes.
</commit_message>
<xml_diff>
--- a/_notes_/Athasian Skill Changes.xlsx
+++ b/_notes_/Athasian Skill Changes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
   <si>
     <t>Class</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Wilder</t>
+  </si>
+  <si>
+    <t>Wizard</t>
+  </si>
+  <si>
+    <t>2E Psionicist</t>
   </si>
 </sst>
 </file>
@@ -468,13 +474,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C50" sqref="C50"/>
+      <selection pane="bottomRight" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -745,6 +751,38 @@
       </c>
       <c r="C49" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="B52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="C55" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Athasian Skill Changes.xlsx
</commit_message>
<xml_diff>
--- a/_notes_/Athasian Skill Changes.xlsx
+++ b/_notes_/Athasian Skill Changes.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12855"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Base Classes" sheetId="1" r:id="rId1"/>
+    <sheet name="Prestige Classes" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -477,10 +477,10 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C56" sqref="C56"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>